<commit_message>
Add Greece and fix map
</commit_message>
<xml_diff>
--- a/03 - Interactive Viz/topojson/countries_code.xlsx
+++ b/03 - Interactive Viz/topojson/countries_code.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="340" windowWidth="23700" windowHeight="15120"/>
+    <workbookView xWindow="120" yWindow="0" windowWidth="23700" windowHeight="15120"/>
   </bookViews>
   <sheets>
     <sheet name="countries-20140629" sheetId="1" r:id="rId1"/>
@@ -750,9 +750,6 @@
     <t>Guinée équatoriale</t>
   </si>
   <si>
-    <t>GR</t>
-  </si>
-  <si>
     <t>Greece</t>
   </si>
   <si>
@@ -2023,6 +2020,9 @@
   </si>
   <si>
     <t>Russia</t>
+  </si>
+  <si>
+    <t>EL</t>
   </si>
 </sst>
 </file>
@@ -2853,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="B192" sqref="B192"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3708,7 +3708,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B78" t="s">
         <v>211</v>
@@ -3840,1773 +3840,1773 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
+        <v>667</v>
+      </c>
+      <c r="B90" t="s">
         <v>243</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>244</v>
-      </c>
-      <c r="C90" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
+        <v>245</v>
+      </c>
+      <c r="B91" t="s">
         <v>246</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>247</v>
-      </c>
-      <c r="C91" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>248</v>
+      </c>
+      <c r="B92" t="s">
         <v>249</v>
       </c>
-      <c r="B92" t="s">
-        <v>250</v>
-      </c>
       <c r="C92" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
+        <v>250</v>
+      </c>
+      <c r="B93" t="s">
         <v>251</v>
       </c>
-      <c r="B93" t="s">
-        <v>252</v>
-      </c>
       <c r="C93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
+        <v>252</v>
+      </c>
+      <c r="B94" t="s">
         <v>253</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>254</v>
-      </c>
-      <c r="C94" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
+        <v>255</v>
+      </c>
+      <c r="B95" t="s">
         <v>256</v>
       </c>
-      <c r="B95" t="s">
-        <v>257</v>
-      </c>
       <c r="C95" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
+        <v>257</v>
+      </c>
+      <c r="B96" t="s">
         <v>258</v>
       </c>
-      <c r="B96" t="s">
-        <v>259</v>
-      </c>
       <c r="C96" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
+        <v>259</v>
+      </c>
+      <c r="B97" t="s">
         <v>260</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>261</v>
-      </c>
-      <c r="C97" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
+        <v>262</v>
+      </c>
+      <c r="B98" t="s">
         <v>263</v>
       </c>
-      <c r="B98" t="s">
-        <v>264</v>
-      </c>
       <c r="C98" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
+        <v>264</v>
+      </c>
+      <c r="B99" t="s">
         <v>265</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>266</v>
-      </c>
-      <c r="C99" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
+        <v>267</v>
+      </c>
+      <c r="B100" t="s">
         <v>268</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>269</v>
-      </c>
-      <c r="C100" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
+        <v>270</v>
+      </c>
+      <c r="B101" t="s">
         <v>271</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>272</v>
-      </c>
-      <c r="C101" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
+        <v>273</v>
+      </c>
+      <c r="B102" t="s">
         <v>274</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>275</v>
-      </c>
-      <c r="C102" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
+        <v>276</v>
+      </c>
+      <c r="B103" t="s">
         <v>277</v>
       </c>
-      <c r="B103" t="s">
+      <c r="C103" t="s">
         <v>278</v>
-      </c>
-      <c r="C103" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
+        <v>279</v>
+      </c>
+      <c r="B104" t="s">
         <v>280</v>
       </c>
-      <c r="B104" t="s">
+      <c r="C104" t="s">
         <v>281</v>
-      </c>
-      <c r="C104" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
+        <v>282</v>
+      </c>
+      <c r="B105" t="s">
         <v>283</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>284</v>
-      </c>
-      <c r="C105" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
+        <v>285</v>
+      </c>
+      <c r="B106" t="s">
         <v>286</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>287</v>
-      </c>
-      <c r="C106" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
+        <v>288</v>
+      </c>
+      <c r="B107" t="s">
         <v>289</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>290</v>
-      </c>
-      <c r="C107" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
+        <v>291</v>
+      </c>
+      <c r="B108" t="s">
         <v>292</v>
       </c>
-      <c r="B108" t="s">
+      <c r="C108" t="s">
         <v>293</v>
-      </c>
-      <c r="C108" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
+        <v>294</v>
+      </c>
+      <c r="B109" t="s">
         <v>295</v>
       </c>
-      <c r="B109" t="s">
-        <v>296</v>
-      </c>
       <c r="C109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
+        <v>296</v>
+      </c>
+      <c r="B110" t="s">
         <v>297</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>298</v>
-      </c>
-      <c r="C110" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
+        <v>299</v>
+      </c>
+      <c r="B111" t="s">
         <v>300</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>301</v>
-      </c>
-      <c r="C111" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
+        <v>302</v>
+      </c>
+      <c r="B112" t="s">
         <v>303</v>
       </c>
-      <c r="B112" t="s">
-        <v>304</v>
-      </c>
       <c r="C112" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
+        <v>304</v>
+      </c>
+      <c r="B113" t="s">
         <v>305</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>306</v>
-      </c>
-      <c r="C113" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
+        <v>307</v>
+      </c>
+      <c r="B114" t="s">
         <v>308</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>309</v>
-      </c>
-      <c r="C114" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
+        <v>310</v>
+      </c>
+      <c r="B115" t="s">
         <v>311</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>312</v>
-      </c>
-      <c r="C115" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>313</v>
+      </c>
+      <c r="B116" t="s">
         <v>314</v>
       </c>
-      <c r="B116" t="s">
-        <v>315</v>
-      </c>
       <c r="C116" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
+        <v>315</v>
+      </c>
+      <c r="B117" t="s">
         <v>316</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>317</v>
-      </c>
-      <c r="C117" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
+        <v>318</v>
+      </c>
+      <c r="B118" t="s">
         <v>319</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>320</v>
-      </c>
-      <c r="C118" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
+        <v>321</v>
+      </c>
+      <c r="B119" t="s">
         <v>322</v>
       </c>
-      <c r="B119" t="s">
-        <v>323</v>
-      </c>
       <c r="C119" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
+        <v>323</v>
+      </c>
+      <c r="B120" t="s">
         <v>324</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>325</v>
-      </c>
-      <c r="C120" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
+        <v>326</v>
+      </c>
+      <c r="B121" t="s">
         <v>327</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>328</v>
-      </c>
-      <c r="C121" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
+        <v>329</v>
+      </c>
+      <c r="B122" t="s">
         <v>330</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>331</v>
-      </c>
-      <c r="C122" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
+        <v>332</v>
+      </c>
+      <c r="B123" t="s">
         <v>333</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>334</v>
-      </c>
-      <c r="C123" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
+        <v>335</v>
+      </c>
+      <c r="B124" t="s">
         <v>336</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>337</v>
-      </c>
-      <c r="C124" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
+        <v>338</v>
+      </c>
+      <c r="B125" t="s">
         <v>339</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>340</v>
-      </c>
-      <c r="C125" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
+        <v>341</v>
+      </c>
+      <c r="B126" t="s">
         <v>342</v>
       </c>
-      <c r="B126" t="s">
-        <v>343</v>
-      </c>
       <c r="C126" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
+        <v>343</v>
+      </c>
+      <c r="B127" t="s">
         <v>344</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>345</v>
-      </c>
-      <c r="C127" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
+        <v>346</v>
+      </c>
+      <c r="B128" t="s">
         <v>347</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>348</v>
-      </c>
-      <c r="C128" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
+        <v>349</v>
+      </c>
+      <c r="B129" t="s">
         <v>350</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>351</v>
-      </c>
-      <c r="C129" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
+        <v>352</v>
+      </c>
+      <c r="B130" t="s">
         <v>353</v>
       </c>
-      <c r="B130" t="s">
-        <v>354</v>
-      </c>
       <c r="C130" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
+        <v>354</v>
+      </c>
+      <c r="B131" t="s">
         <v>355</v>
       </c>
-      <c r="B131" t="s">
-        <v>356</v>
-      </c>
       <c r="C131" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
+        <v>356</v>
+      </c>
+      <c r="B132" t="s">
         <v>357</v>
       </c>
-      <c r="B132" t="s">
+      <c r="C132" t="s">
         <v>358</v>
-      </c>
-      <c r="C132" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
+        <v>359</v>
+      </c>
+      <c r="B133" t="s">
         <v>360</v>
       </c>
-      <c r="B133" t="s">
-        <v>361</v>
-      </c>
       <c r="C133" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
+        <v>361</v>
+      </c>
+      <c r="B134" t="s">
         <v>362</v>
       </c>
-      <c r="B134" t="s">
+      <c r="C134" t="s">
         <v>363</v>
-      </c>
-      <c r="C134" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
+        <v>364</v>
+      </c>
+      <c r="B135" t="s">
         <v>365</v>
       </c>
-      <c r="B135" t="s">
-        <v>366</v>
-      </c>
       <c r="C135" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>366</v>
+      </c>
+      <c r="B136" t="s">
         <v>367</v>
       </c>
-      <c r="B136" t="s">
+      <c r="C136" t="s">
         <v>368</v>
-      </c>
-      <c r="C136" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
+        <v>369</v>
+      </c>
+      <c r="B137" t="s">
         <v>370</v>
       </c>
-      <c r="B137" t="s">
+      <c r="C137" t="s">
         <v>371</v>
-      </c>
-      <c r="C137" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
+        <v>372</v>
+      </c>
+      <c r="B138" t="s">
         <v>373</v>
       </c>
-      <c r="B138" t="s">
+      <c r="C138" t="s">
         <v>374</v>
-      </c>
-      <c r="C138" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
+        <v>375</v>
+      </c>
+      <c r="B139" t="s">
         <v>376</v>
       </c>
-      <c r="B139" t="s">
-        <v>377</v>
-      </c>
       <c r="C139" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
+        <v>377</v>
+      </c>
+      <c r="B140" t="s">
+        <v>664</v>
+      </c>
+      <c r="C140" t="s">
         <v>378</v>
-      </c>
-      <c r="B140" t="s">
-        <v>665</v>
-      </c>
-      <c r="C140" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
+        <v>379</v>
+      </c>
+      <c r="B141" t="s">
         <v>380</v>
       </c>
-      <c r="B141" t="s">
+      <c r="C141" t="s">
         <v>381</v>
-      </c>
-      <c r="C141" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
+        <v>382</v>
+      </c>
+      <c r="B142" t="s">
         <v>383</v>
       </c>
-      <c r="B142" t="s">
-        <v>384</v>
-      </c>
       <c r="C142" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
+        <v>384</v>
+      </c>
+      <c r="B143" t="s">
         <v>385</v>
       </c>
-      <c r="B143" t="s">
-        <v>386</v>
-      </c>
       <c r="C143" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
+        <v>386</v>
+      </c>
+      <c r="B144" t="s">
         <v>387</v>
       </c>
-      <c r="B144" t="s">
+      <c r="C144" t="s">
         <v>388</v>
-      </c>
-      <c r="C144" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
+        <v>389</v>
+      </c>
+      <c r="B145" t="s">
+        <v>661</v>
+      </c>
+      <c r="C145" t="s">
         <v>390</v>
-      </c>
-      <c r="B145" t="s">
-        <v>662</v>
-      </c>
-      <c r="C145" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
+        <v>391</v>
+      </c>
+      <c r="B146" t="s">
         <v>392</v>
       </c>
-      <c r="B146" t="s">
-        <v>393</v>
-      </c>
       <c r="C146" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
+        <v>393</v>
+      </c>
+      <c r="B147" t="s">
         <v>394</v>
       </c>
-      <c r="B147" t="s">
-        <v>395</v>
-      </c>
       <c r="C147" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
+        <v>395</v>
+      </c>
+      <c r="B148" t="s">
         <v>396</v>
       </c>
-      <c r="B148" t="s">
+      <c r="C148" t="s">
         <v>397</v>
-      </c>
-      <c r="C148" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
+        <v>398</v>
+      </c>
+      <c r="B149" t="s">
         <v>399</v>
       </c>
-      <c r="B149" t="s">
+      <c r="C149" t="s">
         <v>400</v>
-      </c>
-      <c r="C149" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
+        <v>401</v>
+      </c>
+      <c r="B150" t="s">
         <v>402</v>
       </c>
-      <c r="B150" t="s">
+      <c r="C150" t="s">
         <v>403</v>
-      </c>
-      <c r="C150" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
+        <v>404</v>
+      </c>
+      <c r="B151" t="s">
         <v>405</v>
       </c>
-      <c r="B151" t="s">
-        <v>406</v>
-      </c>
       <c r="C151" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
+        <v>406</v>
+      </c>
+      <c r="B152" t="s">
         <v>407</v>
       </c>
-      <c r="B152" t="s">
+      <c r="C152" t="s">
         <v>408</v>
-      </c>
-      <c r="C152" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
+        <v>409</v>
+      </c>
+      <c r="B153" t="s">
         <v>410</v>
       </c>
-      <c r="B153" t="s">
-        <v>411</v>
-      </c>
       <c r="C153" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
+        <v>411</v>
+      </c>
+      <c r="B154" t="s">
         <v>412</v>
       </c>
-      <c r="B154" t="s">
+      <c r="C154" t="s">
         <v>413</v>
-      </c>
-      <c r="C154" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
+        <v>414</v>
+      </c>
+      <c r="B155" t="s">
         <v>415</v>
       </c>
-      <c r="B155" t="s">
+      <c r="C155" t="s">
         <v>416</v>
-      </c>
-      <c r="C155" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
+        <v>417</v>
+      </c>
+      <c r="B156" t="s">
         <v>418</v>
       </c>
-      <c r="B156" t="s">
-        <v>419</v>
-      </c>
       <c r="C156" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
+        <v>419</v>
+      </c>
+      <c r="B157" t="s">
         <v>420</v>
       </c>
-      <c r="B157" t="s">
-        <v>421</v>
-      </c>
       <c r="C157" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
+        <v>421</v>
+      </c>
+      <c r="B158" t="s">
         <v>422</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
         <v>423</v>
-      </c>
-      <c r="C158" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
+        <v>424</v>
+      </c>
+      <c r="B159" t="s">
         <v>425</v>
       </c>
-      <c r="B159" t="s">
+      <c r="C159" t="s">
         <v>426</v>
-      </c>
-      <c r="C159" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
+        <v>427</v>
+      </c>
+      <c r="B160" t="s">
         <v>428</v>
       </c>
-      <c r="B160" t="s">
-        <v>429</v>
-      </c>
       <c r="C160" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
+        <v>429</v>
+      </c>
+      <c r="B161" t="s">
         <v>430</v>
       </c>
-      <c r="B161" t="s">
+      <c r="C161" t="s">
         <v>431</v>
-      </c>
-      <c r="C161" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
+        <v>432</v>
+      </c>
+      <c r="B162" t="s">
         <v>433</v>
       </c>
-      <c r="B162" t="s">
+      <c r="C162" t="s">
         <v>434</v>
-      </c>
-      <c r="C162" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
+        <v>435</v>
+      </c>
+      <c r="B163" t="s">
         <v>436</v>
       </c>
-      <c r="B163" t="s">
-        <v>437</v>
-      </c>
       <c r="C163" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
+        <v>437</v>
+      </c>
+      <c r="B164" t="s">
         <v>438</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" t="s">
         <v>439</v>
-      </c>
-      <c r="C164" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
+        <v>440</v>
+      </c>
+      <c r="B165" t="s">
         <v>441</v>
       </c>
-      <c r="B165" t="s">
-        <v>442</v>
-      </c>
       <c r="C165" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
+        <v>442</v>
+      </c>
+      <c r="B166" t="s">
         <v>443</v>
       </c>
-      <c r="B166" t="s">
-        <v>444</v>
-      </c>
       <c r="C166" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
+        <v>444</v>
+      </c>
+      <c r="B167" t="s">
+        <v>663</v>
+      </c>
+      <c r="C167" t="s">
         <v>445</v>
-      </c>
-      <c r="B167" t="s">
-        <v>664</v>
-      </c>
-      <c r="C167" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
+        <v>446</v>
+      </c>
+      <c r="B168" t="s">
         <v>447</v>
       </c>
-      <c r="B168" t="s">
+      <c r="C168" t="s">
         <v>448</v>
-      </c>
-      <c r="C168" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
+        <v>449</v>
+      </c>
+      <c r="B169" t="s">
         <v>450</v>
       </c>
-      <c r="B169" t="s">
+      <c r="C169" t="s">
         <v>451</v>
-      </c>
-      <c r="C169" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
+        <v>452</v>
+      </c>
+      <c r="B170" t="s">
         <v>453</v>
       </c>
-      <c r="B170" t="s">
-        <v>454</v>
-      </c>
       <c r="C170" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
+        <v>454</v>
+      </c>
+      <c r="B171" t="s">
         <v>455</v>
       </c>
-      <c r="B171" t="s">
-        <v>456</v>
-      </c>
       <c r="C171" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
+        <v>456</v>
+      </c>
+      <c r="B172" t="s">
         <v>457</v>
       </c>
-      <c r="B172" t="s">
+      <c r="C172" t="s">
         <v>458</v>
-      </c>
-      <c r="C172" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
+        <v>459</v>
+      </c>
+      <c r="B173" t="s">
         <v>460</v>
       </c>
-      <c r="B173" t="s">
-        <v>461</v>
-      </c>
       <c r="C173" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
+        <v>461</v>
+      </c>
+      <c r="B174" t="s">
         <v>462</v>
       </c>
-      <c r="B174" t="s">
-        <v>463</v>
-      </c>
       <c r="C174" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
+        <v>463</v>
+      </c>
+      <c r="B175" t="s">
         <v>464</v>
       </c>
-      <c r="B175" t="s">
+      <c r="C175" t="s">
         <v>465</v>
-      </c>
-      <c r="C175" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
+        <v>466</v>
+      </c>
+      <c r="B176" t="s">
         <v>467</v>
       </c>
-      <c r="B176" t="s">
+      <c r="C176" t="s">
         <v>468</v>
-      </c>
-      <c r="C176" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
+        <v>469</v>
+      </c>
+      <c r="B177" t="s">
         <v>470</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" t="s">
         <v>471</v>
-      </c>
-      <c r="C177" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
+        <v>472</v>
+      </c>
+      <c r="B178" t="s">
         <v>473</v>
       </c>
-      <c r="B178" t="s">
-        <v>474</v>
-      </c>
       <c r="C178" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
+        <v>474</v>
+      </c>
+      <c r="B179" t="s">
         <v>475</v>
       </c>
-      <c r="B179" t="s">
-        <v>476</v>
-      </c>
       <c r="C179" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
+        <v>476</v>
+      </c>
+      <c r="B180" t="s">
         <v>477</v>
       </c>
-      <c r="B180" t="s">
+      <c r="C180" t="s">
         <v>478</v>
-      </c>
-      <c r="C180" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
+        <v>479</v>
+      </c>
+      <c r="B181" t="s">
         <v>480</v>
       </c>
-      <c r="B181" t="s">
+      <c r="C181" t="s">
         <v>481</v>
-      </c>
-      <c r="C181" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
+        <v>482</v>
+      </c>
+      <c r="B182" t="s">
         <v>483</v>
       </c>
-      <c r="B182" t="s">
-        <v>484</v>
-      </c>
       <c r="C182" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
+        <v>484</v>
+      </c>
+      <c r="B183" t="s">
         <v>485</v>
       </c>
-      <c r="B183" t="s">
-        <v>486</v>
-      </c>
       <c r="C183" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
+        <v>486</v>
+      </c>
+      <c r="B184" t="s">
         <v>487</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C184" t="s">
         <v>488</v>
-      </c>
-      <c r="C184" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
+        <v>489</v>
+      </c>
+      <c r="B185" t="s">
         <v>490</v>
       </c>
-      <c r="B185" t="s">
-        <v>491</v>
-      </c>
       <c r="C185" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
+        <v>491</v>
+      </c>
+      <c r="B186" t="s">
         <v>492</v>
       </c>
-      <c r="B186" t="s">
-        <v>493</v>
-      </c>
       <c r="C186" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
+        <v>493</v>
+      </c>
+      <c r="B187" t="s">
         <v>494</v>
       </c>
-      <c r="B187" t="s">
-        <v>495</v>
-      </c>
       <c r="C187" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
+        <v>495</v>
+      </c>
+      <c r="B188" t="s">
         <v>496</v>
       </c>
-      <c r="B188" t="s">
-        <v>497</v>
-      </c>
       <c r="C188" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
+        <v>497</v>
+      </c>
+      <c r="B189" t="s">
         <v>498</v>
       </c>
-      <c r="B189" t="s">
-        <v>499</v>
-      </c>
       <c r="C189" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
+        <v>499</v>
+      </c>
+      <c r="B190" t="s">
         <v>500</v>
       </c>
-      <c r="B190" t="s">
+      <c r="C190" t="s">
         <v>501</v>
-      </c>
-      <c r="C190" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
+        <v>502</v>
+      </c>
+      <c r="B191" t="s">
         <v>503</v>
       </c>
-      <c r="B191" t="s">
+      <c r="C191" t="s">
         <v>504</v>
-      </c>
-      <c r="C191" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
+        <v>505</v>
+      </c>
+      <c r="B192" t="s">
+        <v>666</v>
+      </c>
+      <c r="C192" t="s">
         <v>506</v>
-      </c>
-      <c r="B192" t="s">
-        <v>667</v>
-      </c>
-      <c r="C192" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
+        <v>507</v>
+      </c>
+      <c r="B193" t="s">
         <v>508</v>
       </c>
-      <c r="B193" t="s">
-        <v>509</v>
-      </c>
       <c r="C193" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
+        <v>509</v>
+      </c>
+      <c r="B194" t="s">
         <v>510</v>
       </c>
-      <c r="B194" t="s">
+      <c r="C194" t="s">
         <v>511</v>
-      </c>
-      <c r="C194" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
+        <v>512</v>
+      </c>
+      <c r="B195" t="s">
         <v>513</v>
       </c>
-      <c r="B195" t="s">
+      <c r="C195" t="s">
         <v>514</v>
-      </c>
-      <c r="C195" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
+        <v>515</v>
+      </c>
+      <c r="B196" t="s">
         <v>516</v>
       </c>
-      <c r="B196" t="s">
-        <v>517</v>
-      </c>
       <c r="C196" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
+        <v>517</v>
+      </c>
+      <c r="B197" t="s">
         <v>518</v>
       </c>
-      <c r="B197" t="s">
+      <c r="C197" t="s">
         <v>519</v>
-      </c>
-      <c r="C197" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
+        <v>520</v>
+      </c>
+      <c r="B198" t="s">
         <v>521</v>
       </c>
-      <c r="B198" t="s">
+      <c r="C198" t="s">
         <v>522</v>
-      </c>
-      <c r="C198" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
+        <v>523</v>
+      </c>
+      <c r="B199" t="s">
         <v>524</v>
       </c>
-      <c r="B199" t="s">
+      <c r="C199" t="s">
         <v>525</v>
-      </c>
-      <c r="C199" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
+        <v>526</v>
+      </c>
+      <c r="B200" t="s">
         <v>527</v>
       </c>
-      <c r="B200" t="s">
+      <c r="C200" t="s">
         <v>528</v>
-      </c>
-      <c r="C200" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
+        <v>529</v>
+      </c>
+      <c r="B201" t="s">
         <v>530</v>
       </c>
-      <c r="B201" t="s">
+      <c r="C201" t="s">
         <v>531</v>
-      </c>
-      <c r="C201" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
+        <v>532</v>
+      </c>
+      <c r="B202" t="s">
         <v>533</v>
       </c>
-      <c r="B202" t="s">
+      <c r="C202" t="s">
         <v>534</v>
-      </c>
-      <c r="C202" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
+        <v>535</v>
+      </c>
+      <c r="B203" t="s">
         <v>536</v>
       </c>
-      <c r="B203" t="s">
+      <c r="C203" t="s">
         <v>537</v>
-      </c>
-      <c r="C203" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
+        <v>538</v>
+      </c>
+      <c r="B204" t="s">
         <v>539</v>
       </c>
-      <c r="B204" t="s">
-        <v>540</v>
-      </c>
       <c r="C204" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
+        <v>540</v>
+      </c>
+      <c r="B205" t="s">
         <v>541</v>
       </c>
-      <c r="B205" t="s">
+      <c r="C205" t="s">
         <v>542</v>
-      </c>
-      <c r="C205" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
+        <v>543</v>
+      </c>
+      <c r="B206" t="s">
         <v>544</v>
       </c>
-      <c r="B206" t="s">
+      <c r="C206" t="s">
         <v>545</v>
-      </c>
-      <c r="C206" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
+        <v>546</v>
+      </c>
+      <c r="B207" t="s">
         <v>547</v>
       </c>
-      <c r="B207" t="s">
+      <c r="C207" t="s">
         <v>548</v>
-      </c>
-      <c r="C207" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
+        <v>549</v>
+      </c>
+      <c r="B208" t="s">
         <v>550</v>
       </c>
-      <c r="B208" t="s">
-        <v>551</v>
-      </c>
       <c r="C208" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
+        <v>551</v>
+      </c>
+      <c r="B209" t="s">
         <v>552</v>
       </c>
-      <c r="B209" t="s">
+      <c r="C209" t="s">
         <v>553</v>
-      </c>
-      <c r="C209" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
+        <v>554</v>
+      </c>
+      <c r="B210" t="s">
         <v>555</v>
       </c>
-      <c r="B210" t="s">
+      <c r="C210" t="s">
         <v>556</v>
-      </c>
-      <c r="C210" t="s">
-        <v>557</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
+        <v>557</v>
+      </c>
+      <c r="B211" t="s">
         <v>558</v>
       </c>
-      <c r="B211" t="s">
-        <v>559</v>
-      </c>
       <c r="C211" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
+        <v>559</v>
+      </c>
+      <c r="B212" t="s">
         <v>560</v>
       </c>
-      <c r="B212" t="s">
+      <c r="C212" t="s">
         <v>561</v>
-      </c>
-      <c r="C212" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
+        <v>562</v>
+      </c>
+      <c r="B213" t="s">
         <v>563</v>
       </c>
-      <c r="B213" t="s">
+      <c r="C213" t="s">
         <v>564</v>
-      </c>
-      <c r="C213" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
+        <v>565</v>
+      </c>
+      <c r="B214" t="s">
         <v>566</v>
       </c>
-      <c r="B214" t="s">
-        <v>567</v>
-      </c>
       <c r="C214" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
+        <v>567</v>
+      </c>
+      <c r="B215" t="s">
         <v>568</v>
       </c>
-      <c r="B215" t="s">
+      <c r="C215" t="s">
         <v>569</v>
-      </c>
-      <c r="C215" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
+        <v>570</v>
+      </c>
+      <c r="B216" t="s">
         <v>571</v>
       </c>
-      <c r="B216" t="s">
+      <c r="C216" t="s">
         <v>572</v>
-      </c>
-      <c r="C216" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
+        <v>573</v>
+      </c>
+      <c r="B217" t="s">
         <v>574</v>
       </c>
-      <c r="B217" t="s">
+      <c r="C217" t="s">
         <v>575</v>
-      </c>
-      <c r="C217" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
+        <v>576</v>
+      </c>
+      <c r="B218" t="s">
         <v>577</v>
       </c>
-      <c r="B218" t="s">
-        <v>578</v>
-      </c>
       <c r="C218" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
+        <v>578</v>
+      </c>
+      <c r="B219" t="s">
         <v>579</v>
       </c>
-      <c r="B219" t="s">
+      <c r="C219" t="s">
         <v>580</v>
-      </c>
-      <c r="C219" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
+        <v>581</v>
+      </c>
+      <c r="B220" t="s">
         <v>582</v>
       </c>
-      <c r="B220" t="s">
+      <c r="C220" t="s">
         <v>583</v>
-      </c>
-      <c r="C220" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
+        <v>584</v>
+      </c>
+      <c r="B221" t="s">
         <v>585</v>
       </c>
-      <c r="B221" t="s">
-        <v>586</v>
-      </c>
       <c r="C221" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
+        <v>586</v>
+      </c>
+      <c r="B222" t="s">
         <v>587</v>
       </c>
-      <c r="B222" t="s">
-        <v>588</v>
-      </c>
       <c r="C222" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
+        <v>588</v>
+      </c>
+      <c r="B223" t="s">
         <v>589</v>
       </c>
-      <c r="B223" t="s">
+      <c r="C223" t="s">
         <v>590</v>
-      </c>
-      <c r="C223" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
+        <v>591</v>
+      </c>
+      <c r="B224" t="s">
         <v>592</v>
       </c>
-      <c r="B224" t="s">
+      <c r="C224" t="s">
         <v>593</v>
-      </c>
-      <c r="C224" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
+        <v>594</v>
+      </c>
+      <c r="B225" t="s">
         <v>595</v>
       </c>
-      <c r="B225" t="s">
-        <v>596</v>
-      </c>
       <c r="C225" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
+        <v>596</v>
+      </c>
+      <c r="B226" t="s">
         <v>597</v>
       </c>
-      <c r="B226" t="s">
+      <c r="C226" t="s">
         <v>598</v>
-      </c>
-      <c r="C226" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
+        <v>599</v>
+      </c>
+      <c r="B227" t="s">
         <v>600</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" t="s">
         <v>601</v>
-      </c>
-      <c r="C227" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
+        <v>602</v>
+      </c>
+      <c r="B228" t="s">
         <v>603</v>
       </c>
-      <c r="B228" t="s">
-        <v>604</v>
-      </c>
       <c r="C228" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
+        <v>604</v>
+      </c>
+      <c r="B229" t="s">
         <v>605</v>
       </c>
-      <c r="B229" t="s">
+      <c r="C229" t="s">
         <v>606</v>
-      </c>
-      <c r="C229" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
+        <v>607</v>
+      </c>
+      <c r="B230" t="s">
         <v>608</v>
       </c>
-      <c r="B230" t="s">
+      <c r="C230" t="s">
         <v>609</v>
-      </c>
-      <c r="C230" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
+        <v>610</v>
+      </c>
+      <c r="B231" t="s">
         <v>611</v>
       </c>
-      <c r="B231" t="s">
-        <v>612</v>
-      </c>
       <c r="C231" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
+        <v>612</v>
+      </c>
+      <c r="B232" t="s">
         <v>613</v>
       </c>
-      <c r="B232" t="s">
+      <c r="C232" t="s">
         <v>614</v>
-      </c>
-      <c r="C232" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
+        <v>615</v>
+      </c>
+      <c r="B233" t="s">
         <v>616</v>
       </c>
-      <c r="B233" t="s">
+      <c r="C233" t="s">
         <v>617</v>
-      </c>
-      <c r="C233" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
+        <v>618</v>
+      </c>
+      <c r="B234" t="s">
         <v>619</v>
       </c>
-      <c r="B234" t="s">
+      <c r="C234" t="s">
         <v>620</v>
-      </c>
-      <c r="C234" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
+        <v>621</v>
+      </c>
+      <c r="B235" t="s">
         <v>622</v>
       </c>
-      <c r="B235" t="s">
-        <v>623</v>
-      </c>
       <c r="C235" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
+        <v>623</v>
+      </c>
+      <c r="B236" t="s">
         <v>624</v>
       </c>
-      <c r="B236" t="s">
+      <c r="C236" t="s">
         <v>625</v>
-      </c>
-      <c r="C236" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
+        <v>626</v>
+      </c>
+      <c r="B237" t="s">
+        <v>665</v>
+      </c>
+      <c r="C237" t="s">
         <v>627</v>
-      </c>
-      <c r="B237" t="s">
-        <v>666</v>
-      </c>
-      <c r="C237" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
+        <v>628</v>
+      </c>
+      <c r="B238" t="s">
         <v>629</v>
       </c>
-      <c r="B238" t="s">
+      <c r="C238" t="s">
         <v>630</v>
-      </c>
-      <c r="C238" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
+        <v>631</v>
+      </c>
+      <c r="B239" t="s">
         <v>632</v>
       </c>
-      <c r="B239" t="s">
-        <v>633</v>
-      </c>
       <c r="C239" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
+        <v>633</v>
+      </c>
+      <c r="B240" t="s">
         <v>634</v>
       </c>
-      <c r="B240" t="s">
+      <c r="C240" t="s">
         <v>635</v>
-      </c>
-      <c r="C240" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
+        <v>636</v>
+      </c>
+      <c r="B241" t="s">
         <v>637</v>
       </c>
-      <c r="B241" t="s">
+      <c r="C241" t="s">
         <v>638</v>
-      </c>
-      <c r="C241" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
+        <v>639</v>
+      </c>
+      <c r="B242" t="s">
         <v>640</v>
       </c>
-      <c r="B242" t="s">
-        <v>641</v>
-      </c>
       <c r="C242" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
+        <v>641</v>
+      </c>
+      <c r="B243" t="s">
         <v>642</v>
       </c>
-      <c r="B243" t="s">
-        <v>643</v>
-      </c>
       <c r="C243" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
+        <v>643</v>
+      </c>
+      <c r="B244" t="s">
         <v>644</v>
       </c>
-      <c r="B244" t="s">
+      <c r="C244" t="s">
         <v>645</v>
-      </c>
-      <c r="C244" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
+        <v>646</v>
+      </c>
+      <c r="B245" t="s">
         <v>647</v>
       </c>
-      <c r="B245" t="s">
-        <v>648</v>
-      </c>
       <c r="C245" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
+        <v>648</v>
+      </c>
+      <c r="B246" t="s">
         <v>649</v>
       </c>
-      <c r="B246" t="s">
+      <c r="C246" t="s">
         <v>650</v>
-      </c>
-      <c r="C246" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
+        <v>651</v>
+      </c>
+      <c r="B247" t="s">
         <v>652</v>
       </c>
-      <c r="B247" t="s">
-        <v>653</v>
-      </c>
       <c r="C247" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
+        <v>653</v>
+      </c>
+      <c r="B248" t="s">
         <v>654</v>
       </c>
-      <c r="B248" t="s">
+      <c r="C248" t="s">
         <v>655</v>
-      </c>
-      <c r="C248" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
+        <v>656</v>
+      </c>
+      <c r="B249" t="s">
         <v>657</v>
       </c>
-      <c r="B249" t="s">
+      <c r="C249" t="s">
         <v>658</v>
-      </c>
-      <c r="C249" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
+        <v>659</v>
+      </c>
+      <c r="B250" t="s">
         <v>660</v>
       </c>
-      <c r="B250" t="s">
-        <v>661</v>
-      </c>
       <c r="C250" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
   </sheetData>

</xml_diff>